<commit_message>
chore(update-logs): style pre-flight update output; silence duplicate update logs; add exit message
</commit_message>
<xml_diff>
--- a/Names.xlsx
+++ b/Names.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Certificate Generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A75E8E-47D6-483D-8789-F91ACB4CB75A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35224B2D-0C1F-4C23-9E38-23C3EE023C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DD7A3C64-0E70-466B-8083-EDFAABCFA219}"/>
   </bookViews>
@@ -25,12 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Sarry Eldeen Mohamed Faisal</t>
+    <t>sarry eldeen mohamed faisal</t>
+  </si>
+  <si>
+    <t>Mariam hany adli Hassan</t>
   </si>
 </sst>
 </file>
@@ -382,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191C142E-5CC7-462A-A0D0-B9D6B9DB93AD}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A3:A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -403,6 +406,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>